<commit_message>
New simulation results, now reads car name from file name automatically, added new path for overcenterline
</commit_message>
<xml_diff>
--- a/simulation_matrix.xlsx
+++ b/simulation_matrix.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\InjuryVisualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D587FA8-D4BB-4508-A28A-F7269F7BA12B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E797D006-32DB-4241-90B6-C9400AA5216A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="2" r:id="rId1"/>
-    <sheet name="2020" sheetId="3" r:id="rId2"/>
+    <sheet name="2020" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="145">
   <si>
     <t>M50-OS</t>
   </si>
@@ -455,6 +455,12 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>Completed w/ Error</t>
   </si>
 </sst>
 </file>
@@ -2056,14 +2062,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFB27DE-F19B-48B7-907E-7905375F40B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11636695-EC93-4881-965B-D6DBAA52EF19}">
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,7 +2080,9 @@
     <col min="4" max="4" width="11.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="8" width="9.140625" style="4"/>
+    <col min="9" max="9" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2143,10 +2151,10 @@
         <v>44134</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2162,11 +2170,17 @@
       <c r="D4" s="4">
         <v>2</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="5">
+        <v>44149</v>
+      </c>
       <c r="H4" s="9" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2188,6 +2202,12 @@
       <c r="F5" s="5">
         <v>44134</v>
       </c>
+      <c r="H5" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -2242,6 +2262,12 @@
       <c r="D8" s="4">
         <v>2</v>
       </c>
+      <c r="E8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="5">
+        <v>44146</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -2296,6 +2322,12 @@
       <c r="D11" s="4">
         <v>2</v>
       </c>
+      <c r="E11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="5">
+        <v>44149</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -2370,6 +2402,12 @@
       <c r="D15" s="4">
         <v>2</v>
       </c>
+      <c r="E15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="5">
+        <v>44146</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -2384,6 +2422,12 @@
       <c r="D16" s="4">
         <v>2</v>
       </c>
+      <c r="E16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="5">
+        <v>44149</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
@@ -2398,6 +2442,12 @@
       <c r="D17" s="4">
         <v>2</v>
       </c>
+      <c r="E17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="5">
+        <v>44149</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -2412,6 +2462,12 @@
       <c r="D18" s="4">
         <v>2</v>
       </c>
+      <c r="E18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="5">
+        <v>44144</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -2426,6 +2482,12 @@
       <c r="D19" s="4">
         <v>2</v>
       </c>
+      <c r="E19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="5">
+        <v>44146</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
@@ -2440,6 +2502,12 @@
       <c r="D20" s="4">
         <v>2</v>
       </c>
+      <c r="E20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="5">
+        <v>44151</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -2454,6 +2522,12 @@
       <c r="D21" s="4">
         <v>2</v>
       </c>
+      <c r="E21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="5">
+        <v>44151</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -2489,10 +2563,10 @@
         <v>2</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F23" s="5">
-        <v>44132</v>
+        <v>44138</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2509,10 +2583,10 @@
         <v>2</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>141</v>
+        <v>66</v>
       </c>
       <c r="F24" s="5">
-        <v>44131</v>
+        <v>44143</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2528,6 +2602,12 @@
       <c r="D25" s="4">
         <v>2</v>
       </c>
+      <c r="E25" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="5">
+        <v>44146</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
@@ -2542,6 +2622,12 @@
       <c r="D26" s="4">
         <v>2</v>
       </c>
+      <c r="E26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="5">
+        <v>44155</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -2556,6 +2642,12 @@
       <c r="D27" s="4">
         <v>2</v>
       </c>
+      <c r="E27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="5">
+        <v>44156</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
@@ -2591,10 +2683,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F29" s="5">
-        <v>44132</v>
+        <v>44142</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2610,6 +2702,12 @@
       <c r="D30" s="4">
         <v>2</v>
       </c>
+      <c r="E30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="5">
+        <v>44151</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
@@ -2623,6 +2721,12 @@
       </c>
       <c r="D31" s="4">
         <v>2</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="5">
+        <v>44151</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>